<commit_message>
changed layout of users page
</commit_message>
<xml_diff>
--- a/doc/Stories Breakdown 1.xlsx
+++ b/doc/Stories Breakdown 1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -178,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +281,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Candara"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -323,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -367,6 +375,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -746,7 +757,7 @@
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,10 +1101,12 @@
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1"/>
+      <c r="F16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
improve UI layout for post liked view
</commit_message>
<xml_diff>
--- a/doc/Stories Breakdown 1.xlsx
+++ b/doc/Stories Breakdown 1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Functionalitate vizualizare utilizatori inregistrati</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Nou: Integrarea unui provider de autentificare (Google)</t>
+  </si>
+  <si>
+    <t>Distribuire via Gmail</t>
   </si>
 </sst>
 </file>
@@ -387,6 +387,17 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Candara"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -756,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +784,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -785,13 +796,13 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
@@ -811,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
@@ -825,7 +836,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
@@ -834,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>6</v>
@@ -859,7 +870,7 @@
       <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
@@ -869,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
@@ -880,7 +891,7 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
@@ -899,9 +910,9 @@
         <v>9</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
@@ -911,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>5</v>
@@ -922,7 +933,9 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
@@ -982,8 +995,12 @@
       <c r="F10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
@@ -998,11 +1015,13 @@
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>26</v>
+      <c r="F11" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
@@ -1021,9 +1040,9 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
@@ -1075,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
@@ -1096,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>5</v>
@@ -1107,7 +1126,7 @@
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
@@ -1117,16 +1136,18 @@
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>26</v>
+      <c r="F17" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -1136,35 +1157,39 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>26</v>
+      <c r="F18" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>18</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>26</v>
+      <c r="F19" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
@@ -1174,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>5</v>
@@ -1183,19 +1208,21 @@
         <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>5</v>
@@ -1216,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>5</v>
@@ -1227,7 +1254,7 @@
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
@@ -1237,7 +1264,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>25</v>
@@ -1246,9 +1273,9 @@
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
@@ -1258,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>25</v>
@@ -1267,9 +1294,9 @@
         <v>9</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>

</xml_diff>